<commit_message>
communicate with new PLC interface (trigger watchdog, rcv ProzessDataTopics)
</commit_message>
<xml_diff>
--- a/CPS_protokoll.xlsx
+++ b/CPS_protokoll.xlsx
@@ -5,16 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Frame" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="JOB" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="ID" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="struktureIOdata" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="HeaderFlag" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$75</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
@@ -28,18 +28,20 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">JOB!$A$2:$G$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$75</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">ID!$A$1:$D$73</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="271">
   <si>
     <t xml:space="preserve">Int[]</t>
   </si>
@@ -798,6 +800,72 @@
   </si>
   <si>
     <t xml:space="preserve">value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SYNC.ERROR      255     1       different client wants to connect -&gt; only one allowed?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SYNC.ERROR      255     2       connection watchdog to connected client timed out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SYNC.acknowlege 1       1       connection to new client established</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SYNC.acknowlege 1       2       retrigger watchdog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUI → PLC (will be answerd by HEADER_ACKN )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SENDdata.data[0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SYNC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topics depending connection establishing, trigger watchdog, register at topics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONNECT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISCONNECT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRIGGER WATCHDOG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERROR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 → connection to client timed out; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">subscribe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEADER_container</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEADER_SYNC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEADER_LogMessage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEADER_ACKN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEADER_PdataIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEADER_PLCdata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEADER_ERROR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plc → GUI</t>
   </si>
 </sst>
 </file>
@@ -953,17 +1021,14 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1376,26 +1441,26 @@
   </sheetPr>
   <dimension ref="2:35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="R14" activeCellId="0" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.1530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2138,10 +2203,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5663265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3201,7 +3264,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D73"/>
+  <autoFilter ref="A1:D75"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3218,15 +3281,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:B2"/>
+  <dimension ref="A2:E34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.60204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3235,6 +3302,148 @@
       </c>
       <c r="B2" s="0" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>